<commit_message>
added acens and separated offers for acens and colt
</commit_message>
<xml_diff>
--- a/provs/colt/historical data colt.xlsx
+++ b/provs/colt/historical data colt.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18915" windowHeight="11310" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18915" windowHeight="11310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ondemand" sheetId="1" r:id="rId1"/>
     <sheet name="features" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
-    <sheet name="bandwidth" sheetId="4" r:id="rId4"/>
+    <sheet name="pricings1" sheetId="5" r:id="rId3"/>
+    <sheet name="pricings2" sheetId="7" r:id="rId4"/>
+    <sheet name="features2" sheetId="6" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId6"/>
+    <sheet name="bandwidth" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ondemand!$A$1:$H$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">pricings1!$A$1:$H$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">pricings2!$A$1:$H$1</definedName>
     <definedName name="iaas_curent_pricings" localSheetId="0">ondemand!#REF!</definedName>
+    <definedName name="iaas_curent_pricings" localSheetId="2">pricings1!#REF!</definedName>
+    <definedName name="iaas_curent_pricings" localSheetId="3">pricings2!#REF!</definedName>
     <definedName name="iaas_current_pricings" localSheetId="0">ondemand!$A$1:$H$1</definedName>
+    <definedName name="iaas_current_pricings" localSheetId="2">pricings1!$A$1:$H$1</definedName>
+    <definedName name="iaas_current_pricings" localSheetId="3">pricings2!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -40,11 +49,45 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="iaas current pricings11" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="I:\Fortu\CloudStation\s21\cspsim\provs\amazon\iaas current pricings.csv" decimal="," thousands="." tab="0" semicolon="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="iaas current pricings111" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="I:\Fortu\CloudStation\s21\cspsim\provs\amazon\iaas current pricings.csv" decimal="," thousands="." tab="0" semicolon="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -194,17 +237,80 @@
   <si>
     <t>Telvent SOC
 Julio 2012</t>
+  </si>
+  <si>
+    <t>sto (SATA)</t>
+  </si>
+  <si>
+    <t>essential1</t>
+  </si>
+  <si>
+    <t>essential2</t>
+  </si>
+  <si>
+    <t>essential3</t>
+  </si>
+  <si>
+    <t>essential4</t>
+  </si>
+  <si>
+    <t>essential5</t>
+  </si>
+  <si>
+    <t>enterprise1</t>
+  </si>
+  <si>
+    <t>enterprise2</t>
+  </si>
+  <si>
+    <t>enterprise3</t>
+  </si>
+  <si>
+    <t>enterprise4</t>
+  </si>
+  <si>
+    <t>enterprise5</t>
+  </si>
+  <si>
+    <t>essential6</t>
+  </si>
+  <si>
+    <t>essential7</t>
+  </si>
+  <si>
+    <t>essential8</t>
+  </si>
+  <si>
+    <t>essential9</t>
+  </si>
+  <si>
+    <t>essential10</t>
+  </si>
+  <si>
+    <t>enterprise6</t>
+  </si>
+  <si>
+    <t>enterprise7</t>
+  </si>
+  <si>
+    <t>enterprise8</t>
+  </si>
+  <si>
+    <t>enterprise9</t>
+  </si>
+  <si>
+    <t>enterprise10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,24 +460,12 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -439,7 +533,7 @@
             <c:numRef>
               <c:f>bandwidth!$D$2:$D$14</c:f>
               <c:numCache>
-                <c:formatCode>#.##000\ "€"</c:formatCode>
+                <c:formatCode>#,##0.00\ "€"</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
@@ -483,7 +577,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -552,7 +645,7 @@
             <c:numRef>
               <c:f>bandwidth!$E$2:$E$14</c:f>
               <c:numCache>
-                <c:formatCode>#.##000\ "€"</c:formatCode>
+                <c:formatCode>#,##0.00\ "€"</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>46.666666666666671</c:v>
@@ -596,48 +689,34 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="104231680"/>
-        <c:axId val="104233216"/>
+        <c:dLbls/>
+        <c:axId val="145176064"/>
+        <c:axId val="145177984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104231680"/>
+        <c:axId val="145176064"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104233216"/>
+        <c:crossAx val="145177984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104233216"/>
+        <c:axId val="145177984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="#.##000\ &quot;€&quot;" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="#,##0.00\ &quot;€&quot;" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104231680"/>
+        <c:crossAx val="145176064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -645,15 +724,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -696,6 +773,14 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="iaas current pricings" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="iaas current pricings" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="iaas current pricings" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -773,7 +858,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -808,7 +892,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -984,15 +1067,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B11"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="5" customWidth="1"/>
@@ -1002,7 +1085,7 @@
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1117,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1070,7 +1153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -1106,7 +1189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
@@ -1142,7 +1225,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -1178,7 +1261,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
@@ -1214,7 +1297,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -1250,7 +1333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -1286,7 +1369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
@@ -1322,7 +1405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -1358,7 +1441,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -1401,14 +1484,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2:N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="8" customWidth="1"/>
     <col min="2" max="2" width="66.42578125" style="10" customWidth="1"/>
@@ -1427,7 +1510,7 @@
     <col min="15" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1471,7 +1554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
@@ -1502,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
@@ -1533,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="9" t="s">
         <v>28</v>
       </c>
@@ -1564,7 +1647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
@@ -1595,7 +1678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
@@ -1626,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="9" t="s">
         <v>33</v>
       </c>
@@ -1657,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="9" t="s">
         <v>34</v>
       </c>
@@ -1688,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="9" t="s">
         <v>35</v>
       </c>
@@ -1719,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="9" t="s">
         <v>36</v>
       </c>
@@ -1750,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="9" t="s">
         <v>37</v>
       </c>
@@ -1788,16 +1871,1613 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="14" style="17" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="17">
+        <f>(15*$I2+8.5*$J2+0.1*K2)/(30*24)</f>
+        <v>0.40166666666666667</v>
+      </c>
+      <c r="F2" s="17">
+        <f>E2</f>
+        <v>0.40166666666666667</v>
+      </c>
+      <c r="G2" s="17">
+        <f t="shared" ref="G2:H2" si="0">F2</f>
+        <v>0.40166666666666667</v>
+      </c>
+      <c r="H2" s="17">
+        <f t="shared" si="0"/>
+        <v>0.40166666666666667</v>
+      </c>
+      <c r="I2" s="8">
+        <v>4</v>
+      </c>
+      <c r="J2" s="8">
+        <v>25.2</v>
+      </c>
+      <c r="K2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="17">
+        <f t="shared" ref="E3:E11" si="1">(15*$I3+8.5*$J3+0.1*K3)/(30*24)</f>
+        <v>0.54944444444444451</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" ref="F3:H11" si="2">E3</f>
+        <v>0.54944444444444451</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" si="2"/>
+        <v>0.54944444444444451</v>
+      </c>
+      <c r="H3" s="17">
+        <f t="shared" si="2"/>
+        <v>0.54944444444444451</v>
+      </c>
+      <c r="I3" s="8">
+        <v>6</v>
+      </c>
+      <c r="J3" s="8">
+        <v>33.6</v>
+      </c>
+      <c r="K3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="17">
+        <f t="shared" si="1"/>
+        <v>0.69722222222222219</v>
+      </c>
+      <c r="F4" s="17">
+        <f t="shared" si="2"/>
+        <v>0.69722222222222219</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" si="2"/>
+        <v>0.69722222222222219</v>
+      </c>
+      <c r="H4" s="17">
+        <f t="shared" si="2"/>
+        <v>0.69722222222222219</v>
+      </c>
+      <c r="I4" s="8">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8">
+        <v>42</v>
+      </c>
+      <c r="K4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="17">
+        <f t="shared" si="1"/>
+        <v>0.89361111111111113</v>
+      </c>
+      <c r="F5" s="17">
+        <f t="shared" si="2"/>
+        <v>0.89361111111111113</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" si="2"/>
+        <v>0.89361111111111113</v>
+      </c>
+      <c r="H5" s="17">
+        <f t="shared" si="2"/>
+        <v>0.89361111111111113</v>
+      </c>
+      <c r="I5" s="8">
+        <v>12</v>
+      </c>
+      <c r="J5" s="8">
+        <v>50.4</v>
+      </c>
+      <c r="K5">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="17">
+        <f t="shared" si="1"/>
+        <v>1.1465277777777778</v>
+      </c>
+      <c r="F6" s="17">
+        <f t="shared" si="2"/>
+        <v>1.1465277777777778</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="2"/>
+        <v>1.1465277777777778</v>
+      </c>
+      <c r="H6" s="17">
+        <f t="shared" si="2"/>
+        <v>1.1465277777777778</v>
+      </c>
+      <c r="I6" s="8">
+        <v>16</v>
+      </c>
+      <c r="J6" s="8">
+        <v>63</v>
+      </c>
+      <c r="K6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="17">
+        <f t="shared" si="1"/>
+        <v>1.3697222222222223</v>
+      </c>
+      <c r="F7" s="17">
+        <f t="shared" si="2"/>
+        <v>1.3697222222222223</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="2"/>
+        <v>1.3697222222222223</v>
+      </c>
+      <c r="H7" s="17">
+        <f t="shared" si="2"/>
+        <v>1.3697222222222223</v>
+      </c>
+      <c r="I7" s="8">
+        <v>24</v>
+      </c>
+      <c r="J7" s="8">
+        <v>67.2</v>
+      </c>
+      <c r="K7">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="1"/>
+        <v>1.6354166666666667</v>
+      </c>
+      <c r="F8" s="17">
+        <f t="shared" si="2"/>
+        <v>1.6354166666666667</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="2"/>
+        <v>1.6354166666666667</v>
+      </c>
+      <c r="H8" s="17">
+        <f t="shared" si="2"/>
+        <v>1.6354166666666667</v>
+      </c>
+      <c r="I8" s="8">
+        <v>32</v>
+      </c>
+      <c r="J8" s="8">
+        <v>75</v>
+      </c>
+      <c r="K8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" si="1"/>
+        <v>2.0819444444444444</v>
+      </c>
+      <c r="F9" s="17">
+        <f t="shared" si="2"/>
+        <v>2.0819444444444444</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="2"/>
+        <v>2.0819444444444444</v>
+      </c>
+      <c r="H9" s="17">
+        <f t="shared" si="2"/>
+        <v>2.0819444444444444</v>
+      </c>
+      <c r="I9" s="8">
+        <v>48</v>
+      </c>
+      <c r="J9" s="8">
+        <v>84</v>
+      </c>
+      <c r="K9">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="17">
+        <f t="shared" si="1"/>
+        <v>2.4718055555555556</v>
+      </c>
+      <c r="F10" s="17">
+        <f t="shared" si="2"/>
+        <v>2.4718055555555556</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="2"/>
+        <v>2.4718055555555556</v>
+      </c>
+      <c r="H10" s="17">
+        <f t="shared" si="2"/>
+        <v>2.4718055555555556</v>
+      </c>
+      <c r="I10" s="8">
+        <v>64</v>
+      </c>
+      <c r="J10" s="8">
+        <v>88.2</v>
+      </c>
+      <c r="K10">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="1"/>
+        <v>3.3194444444444446</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="2"/>
+        <v>3.3194444444444446</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="2"/>
+        <v>3.3194444444444446</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="2"/>
+        <v>3.3194444444444446</v>
+      </c>
+      <c r="I11" s="8">
+        <v>96</v>
+      </c>
+      <c r="J11" s="8">
+        <v>100</v>
+      </c>
+      <c r="K11">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A2:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="14" style="17" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="17">
+        <f>(25*$I2+25*$J2+0.1*K2)/(30*24)</f>
+        <v>1.0347222222222223</v>
+      </c>
+      <c r="F2" s="17">
+        <f t="shared" ref="F2:H8" si="0">E2</f>
+        <v>1.0347222222222223</v>
+      </c>
+      <c r="G2" s="17">
+        <f t="shared" si="0"/>
+        <v>1.0347222222222223</v>
+      </c>
+      <c r="H2" s="17">
+        <f t="shared" si="0"/>
+        <v>1.0347222222222223</v>
+      </c>
+      <c r="I2" s="8">
+        <v>4</v>
+      </c>
+      <c r="J2" s="8">
+        <v>25.2</v>
+      </c>
+      <c r="K2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="17">
+        <f t="shared" ref="E3:E11" si="1">(25*$I3+25*$J3+0.1*K3)/(30*24)</f>
+        <v>1.4027777777777777</v>
+      </c>
+      <c r="F3" s="17">
+        <f t="shared" si="0"/>
+        <v>1.4027777777777777</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" si="0"/>
+        <v>1.4027777777777777</v>
+      </c>
+      <c r="H3" s="17">
+        <f t="shared" si="0"/>
+        <v>1.4027777777777777</v>
+      </c>
+      <c r="I3" s="8">
+        <v>6</v>
+      </c>
+      <c r="J3" s="8">
+        <v>33.6</v>
+      </c>
+      <c r="K3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="17">
+        <f t="shared" si="1"/>
+        <v>1.7708333333333333</v>
+      </c>
+      <c r="F4" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7708333333333333</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7708333333333333</v>
+      </c>
+      <c r="H4" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7708333333333333</v>
+      </c>
+      <c r="I4" s="8">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8">
+        <v>42</v>
+      </c>
+      <c r="K4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="17">
+        <f t="shared" si="1"/>
+        <v>2.2152777777777777</v>
+      </c>
+      <c r="F5" s="17">
+        <f t="shared" si="0"/>
+        <v>2.2152777777777777</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" si="0"/>
+        <v>2.2152777777777777</v>
+      </c>
+      <c r="H5" s="17">
+        <f t="shared" si="0"/>
+        <v>2.2152777777777777</v>
+      </c>
+      <c r="I5" s="8">
+        <v>12</v>
+      </c>
+      <c r="J5" s="8">
+        <v>50.4</v>
+      </c>
+      <c r="K5">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="17">
+        <f t="shared" si="1"/>
+        <v>2.8125</v>
+      </c>
+      <c r="F6" s="17">
+        <f t="shared" si="0"/>
+        <v>2.8125</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
+        <v>2.8125</v>
+      </c>
+      <c r="H6" s="17">
+        <f t="shared" si="0"/>
+        <v>2.8125</v>
+      </c>
+      <c r="I6" s="8">
+        <v>16</v>
+      </c>
+      <c r="J6" s="8">
+        <v>63</v>
+      </c>
+      <c r="K6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="17">
+        <f t="shared" si="1"/>
+        <v>3.2430555555555554</v>
+      </c>
+      <c r="F7" s="17">
+        <f t="shared" si="0"/>
+        <v>3.2430555555555554</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
+        <v>3.2430555555555554</v>
+      </c>
+      <c r="H7" s="17">
+        <f t="shared" si="0"/>
+        <v>3.2430555555555554</v>
+      </c>
+      <c r="I7" s="8">
+        <v>24</v>
+      </c>
+      <c r="J7" s="8">
+        <v>67.2</v>
+      </c>
+      <c r="K7">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="1"/>
+        <v>3.7986111111111112</v>
+      </c>
+      <c r="F8" s="17">
+        <f t="shared" si="0"/>
+        <v>3.7986111111111112</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>3.7986111111111112</v>
+      </c>
+      <c r="H8" s="17">
+        <f t="shared" si="0"/>
+        <v>3.7986111111111112</v>
+      </c>
+      <c r="I8" s="8">
+        <v>32</v>
+      </c>
+      <c r="J8" s="8">
+        <v>75</v>
+      </c>
+      <c r="K8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" si="1"/>
+        <v>4.6736111111111107</v>
+      </c>
+      <c r="F9" s="17">
+        <f t="shared" ref="F9:H11" si="2">E9</f>
+        <v>4.6736111111111107</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="2"/>
+        <v>4.6736111111111107</v>
+      </c>
+      <c r="H9" s="17">
+        <f t="shared" si="2"/>
+        <v>4.6736111111111107</v>
+      </c>
+      <c r="I9" s="8">
+        <v>48</v>
+      </c>
+      <c r="J9" s="8">
+        <v>84</v>
+      </c>
+      <c r="K9">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="17">
+        <f t="shared" si="1"/>
+        <v>5.3819444444444446</v>
+      </c>
+      <c r="F10" s="17">
+        <f t="shared" si="2"/>
+        <v>5.3819444444444446</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="2"/>
+        <v>5.3819444444444446</v>
+      </c>
+      <c r="H10" s="17">
+        <f t="shared" si="2"/>
+        <v>5.3819444444444446</v>
+      </c>
+      <c r="I10" s="8">
+        <v>64</v>
+      </c>
+      <c r="J10" s="8">
+        <v>88.2</v>
+      </c>
+      <c r="K10">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="1"/>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="2"/>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="2"/>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="2"/>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="I11" s="8">
+        <v>96</v>
+      </c>
+      <c r="J11" s="8">
+        <v>100</v>
+      </c>
+      <c r="K11">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="66.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="8">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8">
+        <f>E2*0.4</f>
+        <v>1.6</v>
+      </c>
+      <c r="I2" s="8">
+        <v>25.2</v>
+      </c>
+      <c r="J2" s="8">
+        <f>I2*0.25</f>
+        <v>6.3</v>
+      </c>
+      <c r="L2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="8">
+        <v>6</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F11" si="0">E3*0.4</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="I3" s="8">
+        <v>33.6</v>
+      </c>
+      <c r="J3" s="8">
+        <f t="shared" ref="J3:J11" si="1">I3*0.25</f>
+        <v>8.4</v>
+      </c>
+      <c r="L3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="8">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="I4" s="8">
+        <v>42</v>
+      </c>
+      <c r="J4" s="8">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="L4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8">
+        <v>12</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="I5" s="8">
+        <v>50.4</v>
+      </c>
+      <c r="J5" s="8">
+        <f t="shared" si="1"/>
+        <v>12.6</v>
+      </c>
+      <c r="L5">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>6.4</v>
+      </c>
+      <c r="I6" s="8">
+        <v>63</v>
+      </c>
+      <c r="J6" s="8">
+        <f t="shared" si="1"/>
+        <v>15.75</v>
+      </c>
+      <c r="L6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="8">
+        <v>24</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="I7" s="8">
+        <v>67.2</v>
+      </c>
+      <c r="J7" s="8">
+        <f t="shared" si="1"/>
+        <v>16.8</v>
+      </c>
+      <c r="L7">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="8">
+        <v>32</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>12.8</v>
+      </c>
+      <c r="I8" s="8">
+        <v>75</v>
+      </c>
+      <c r="J8" s="8">
+        <f t="shared" si="1"/>
+        <v>18.75</v>
+      </c>
+      <c r="L8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="8">
+        <v>48</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>19.200000000000003</v>
+      </c>
+      <c r="I9" s="8">
+        <v>84</v>
+      </c>
+      <c r="J9" s="8">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="L9">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="8">
+        <v>64</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>25.6</v>
+      </c>
+      <c r="I10" s="8">
+        <v>88.2</v>
+      </c>
+      <c r="J10" s="8">
+        <f t="shared" si="1"/>
+        <v>22.05</v>
+      </c>
+      <c r="L10">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="8">
+        <v>96</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>38.400000000000006</v>
+      </c>
+      <c r="I11" s="8">
+        <v>100</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="L11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="8">
+        <v>4</v>
+      </c>
+      <c r="F12" s="8">
+        <f>E12*0.75</f>
+        <v>3</v>
+      </c>
+      <c r="I12" s="8">
+        <v>25.2</v>
+      </c>
+      <c r="J12" s="8">
+        <f>I12*0.75</f>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="L12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="8">
+        <v>6</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" ref="F13:F21" si="2">E13*0.75</f>
+        <v>4.5</v>
+      </c>
+      <c r="I13" s="8">
+        <v>33.6</v>
+      </c>
+      <c r="J13" s="8">
+        <f t="shared" ref="J13:J21" si="3">I13*0.75</f>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="L13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="8">
+        <v>8</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="I14" s="8">
+        <v>42</v>
+      </c>
+      <c r="J14" s="8">
+        <f t="shared" si="3"/>
+        <v>31.5</v>
+      </c>
+      <c r="L14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="8">
+        <v>12</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="I15" s="8">
+        <v>50.4</v>
+      </c>
+      <c r="J15" s="8">
+        <f t="shared" si="3"/>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="L15">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="8">
+        <v>16</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="8">
+        <v>63</v>
+      </c>
+      <c r="J16" s="8">
+        <f t="shared" si="3"/>
+        <v>47.25</v>
+      </c>
+      <c r="L16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="8">
+        <v>24</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="I17" s="8">
+        <v>67.2</v>
+      </c>
+      <c r="J17" s="8">
+        <f t="shared" si="3"/>
+        <v>50.400000000000006</v>
+      </c>
+      <c r="L17">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="8">
+        <v>32</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="I18" s="8">
+        <v>75</v>
+      </c>
+      <c r="J18" s="8">
+        <f t="shared" si="3"/>
+        <v>56.25</v>
+      </c>
+      <c r="L18">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="8">
+        <v>48</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I19" s="8">
+        <v>84</v>
+      </c>
+      <c r="J19" s="8">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="L19">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="8">
+        <v>64</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="I20" s="8">
+        <v>88.2</v>
+      </c>
+      <c r="J20" s="8">
+        <f t="shared" si="3"/>
+        <v>66.150000000000006</v>
+      </c>
+      <c r="L20">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="8">
+        <v>96</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="I21" s="8">
+        <v>100</v>
+      </c>
+      <c r="J21" s="8">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="L21">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1805,7 +3485,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1831,7 +3511,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1842,7 +3522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1873,7 +3553,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1904,7 +3584,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1935,7 +3615,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1966,7 +3646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1997,7 +3677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>15</v>
       </c>
@@ -2005,7 +3685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>20</v>
       </c>
@@ -2013,7 +3693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>25</v>
       </c>
@@ -2021,7 +3701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>30</v>
       </c>
@@ -2029,7 +3709,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>35</v>
       </c>
@@ -2037,7 +3717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>40</v>
       </c>
@@ -2045,7 +3725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>45</v>
       </c>
@@ -2053,7 +3733,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>50</v>
       </c>
@@ -2061,7 +3741,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>55</v>
       </c>
@@ -2069,7 +3749,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>60</v>
       </c>
@@ -2077,7 +3757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>65</v>
       </c>
@@ -2085,7 +3765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>70</v>
       </c>
@@ -2093,7 +3773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>75</v>
       </c>
@@ -2101,7 +3781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>80</v>
       </c>
@@ -2109,7 +3789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>85</v>
       </c>
@@ -2117,7 +3797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>90</v>
       </c>
@@ -2125,7 +3805,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>95</v>
       </c>
@@ -2133,7 +3813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>100</v>
       </c>
@@ -2141,7 +3821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>110</v>
       </c>
@@ -2149,7 +3829,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>120</v>
       </c>
@@ -2157,7 +3837,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>130</v>
       </c>
@@ -2165,7 +3845,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>140</v>
       </c>
@@ -2173,7 +3853,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>150</v>
       </c>
@@ -2181,7 +3861,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>160</v>
       </c>
@@ -2189,7 +3869,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>170</v>
       </c>
@@ -2197,7 +3877,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>180</v>
       </c>
@@ -2205,7 +3885,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>190</v>
       </c>
@@ -2213,7 +3893,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>200</v>
       </c>
@@ -2221,7 +3901,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>210</v>
       </c>
@@ -2229,7 +3909,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>220</v>
       </c>
@@ -2237,7 +3917,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>230</v>
       </c>
@@ -2245,7 +3925,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>240</v>
       </c>
@@ -2253,7 +3933,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>250</v>
       </c>
@@ -2261,7 +3941,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>260</v>
       </c>
@@ -2269,7 +3949,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>270</v>
       </c>
@@ -2277,7 +3957,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>280</v>
       </c>
@@ -2285,7 +3965,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>290</v>
       </c>
@@ -2293,7 +3973,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>300</v>
       </c>
@@ -2301,7 +3981,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>310</v>
       </c>
@@ -2309,7 +3989,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>320</v>
       </c>
@@ -2317,7 +3997,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>330</v>
       </c>
@@ -2325,7 +4005,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>340</v>
       </c>
@@ -2333,7 +4013,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>350</v>
       </c>
@@ -2341,7 +4021,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>360</v>
       </c>
@@ -2349,7 +4029,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>370</v>
       </c>
@@ -2357,7 +4037,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>380</v>
       </c>
@@ -2365,7 +4045,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>390</v>
       </c>
@@ -2373,7 +4053,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>400</v>
       </c>
@@ -2381,7 +4061,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>410</v>
       </c>
@@ -2389,7 +4069,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>420</v>
       </c>
@@ -2397,7 +4077,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>430</v>
       </c>
@@ -2405,7 +4085,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>440</v>
       </c>
@@ -2413,7 +4093,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>450</v>
       </c>
@@ -2421,7 +4101,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>460</v>
       </c>
@@ -2429,7 +4109,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>470</v>
       </c>
@@ -2437,7 +4117,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>480</v>
       </c>
@@ -2445,7 +4125,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>490</v>
       </c>
@@ -2453,7 +4133,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>500</v>
       </c>
@@ -2461,222 +4141,222 @@
         <v>360</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="B67">
         <v>370</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="B68">
         <v>380</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="B69">
         <v>390</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="B70">
         <v>400</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="B71">
         <v>410</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="B72">
         <v>420</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="B73">
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="B74">
         <v>440</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="B75">
         <v>450</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="B76">
         <v>460</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="B77">
         <v>470</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="B78">
         <v>480</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="B79">
         <v>490</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="B80">
         <v>500</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2">
       <c r="B81">
         <v>550</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2">
       <c r="B82">
         <v>600</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2">
       <c r="B83">
         <v>650</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2">
       <c r="B84">
         <v>700</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2">
       <c r="B85">
         <v>750</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2">
       <c r="B86">
         <v>800</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2">
       <c r="B87">
         <v>850</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2">
       <c r="B88">
         <v>900</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2">
       <c r="B89">
         <v>950</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2">
       <c r="B90">
         <v>1000</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2">
       <c r="B91">
         <v>1050</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2">
       <c r="B92">
         <v>1100</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2">
       <c r="B93">
         <v>1150</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2">
       <c r="B94">
         <v>1200</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2">
       <c r="B95">
         <v>1250</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2">
       <c r="B96">
         <v>1300</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2">
       <c r="B97">
         <v>1350</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2">
       <c r="B98">
         <v>1400</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2">
       <c r="B99">
         <v>1450</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2">
       <c r="B100">
         <v>1500</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2">
       <c r="B101">
         <v>1550</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2">
       <c r="B102">
         <v>1600</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2">
       <c r="B103">
         <v>1650</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2">
       <c r="B104">
         <v>1700</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2">
       <c r="B105">
         <v>1750</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2">
       <c r="B106">
         <v>1800</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2">
       <c r="B107">
         <v>1850</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2">
       <c r="B108">
         <v>1900</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2">
       <c r="B109">
         <v>1950</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2">
       <c r="B110">
         <v>2000</v>
       </c>
@@ -2699,21 +4379,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -2731,7 +4411,7 @@
       </c>
       <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2750,7 +4430,7 @@
         <v>46.666666666666671</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>4</v>
       </c>
@@ -2769,7 +4449,7 @@
         <v>63.083333333333336</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>6</v>
       </c>
@@ -2788,7 +4468,7 @@
         <v>63.166666666666671</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>8</v>
       </c>
@@ -2807,7 +4487,7 @@
         <v>63.083333333333336</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>10</v>
       </c>
@@ -2826,7 +4506,7 @@
         <v>63.13333333333334</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>20</v>
       </c>
@@ -2845,7 +4525,7 @@
         <v>71.416666666666657</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>30</v>
       </c>
@@ -2864,7 +4544,7 @@
         <v>66.666666666666657</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>40</v>
       </c>
@@ -2883,7 +4563,7 @@
         <v>64.166666666666657</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>50</v>
       </c>
@@ -2902,7 +4582,7 @@
         <v>61.666666666666664</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>60</v>
       </c>
@@ -2921,7 +4601,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>80</v>
       </c>
@@ -2940,7 +4620,7 @@
         <v>56.041666666666664</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>90</v>
       </c>
@@ -2959,7 +4639,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>100</v>
       </c>
@@ -2978,7 +4658,7 @@
         <v>54.166666666666664</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45">
       <c r="A16">
         <v>4</v>
       </c>
@@ -2989,7 +4669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>23</v>
       </c>

</xml_diff>